<commit_message>
Stand up y tablas
</commit_message>
<xml_diff>
--- a/Semana 26-30 de octubre/Stand_Up_Meeitng_Week_10.xlsx
+++ b/Semana 26-30 de octubre/Stand_Up_Meeitng_Week_10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\GitHub\Ingenieria_Software\Semana 26-30 de octubre\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula\Documents\GitHub\Ingenieria_Software\Semana 26-30 de octubre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89658D27-5EBF-46E5-BA9C-E34249764634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F916AF7-A381-4243-B163-FD3885244177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="708" yWindow="2208" windowWidth="21348" windowHeight="8100" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t xml:space="preserve"> MIEMBRO</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>Coursera</t>
+  </si>
+  <si>
+    <t>Reunión con el profesor, tomamos en cuenta las apreciaciones.</t>
+  </si>
+  <si>
+    <t>Reunión con Guille y Santi para corregir algunos errores</t>
+  </si>
+  <si>
+    <t>Reunión con el profesor, asignación de tareas</t>
+  </si>
+  <si>
+    <t>Asistir a la reunión</t>
+  </si>
+  <si>
+    <t>Correcciones a mi parte de las tablas de casos de uso</t>
+  </si>
+  <si>
+    <t>Correcciones a tablas y diagrama.</t>
   </si>
 </sst>
 </file>
@@ -733,7 +751,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,9 +912,15 @@
       <c r="D10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
@@ -909,9 +933,15 @@
       <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
@@ -924,9 +954,15 @@
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">

</xml_diff>